<commit_message>
running test at home 8
</commit_message>
<xml_diff>
--- a/readexcel_write.xlsx
+++ b/readexcel_write.xlsx
@@ -958,85 +958,85 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>welcome</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>welcome</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>welcome</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>welcome</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>welcome</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>welcome</t>
         </is>

</xml_diff>